<commit_message>
WIP processing list and adding to word pairs and equal pairs
</commit_message>
<xml_diff>
--- a/dźěłowe_wersije/060_sc_sw_marka.tsv_wobdźelane_05.09.2024.xlsx
+++ b/dźěłowe_wersije/060_sc_sw_marka.tsv_wobdźelane_05.09.2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5867" uniqueCount="3215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5949" uniqueCount="3215">
   <si>
     <t xml:space="preserve">na</t>
   </si>
@@ -9674,7 +9674,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -9718,6 +9718,14 @@
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -9790,7 +9798,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -9815,11 +9823,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -9842,8 +9854,8 @@
   </sheetPr>
   <dimension ref="A1:D2866"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B120" activeCellId="0" sqref="B120"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A211" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D224" activeCellId="0" sqref="D224:D228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11815,7 +11827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="n">
         <v>11</v>
       </c>
@@ -11825,8 +11837,11 @@
       <c r="C143" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D143" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="n">
         <v>11</v>
       </c>
@@ -11836,8 +11851,11 @@
       <c r="C144" s="0" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D144" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="n">
         <v>11</v>
       </c>
@@ -11847,8 +11865,11 @@
       <c r="C145" s="0" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D145" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="n">
         <v>11</v>
       </c>
@@ -11858,8 +11879,11 @@
       <c r="C146" s="0" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D146" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="n">
         <v>11</v>
       </c>
@@ -11869,8 +11893,11 @@
       <c r="C147" s="0" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D147" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="n">
         <v>11</v>
       </c>
@@ -11880,8 +11907,11 @@
       <c r="C148" s="0" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D148" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="n">
         <v>11</v>
       </c>
@@ -11891,8 +11921,11 @@
       <c r="C149" s="0" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D149" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
         <v>11</v>
       </c>
@@ -11902,8 +11935,11 @@
       <c r="C150" s="0" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D150" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
         <v>11</v>
       </c>
@@ -11913,8 +11949,11 @@
       <c r="C151" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D151" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
         <v>11</v>
       </c>
@@ -11924,8 +11963,11 @@
       <c r="C152" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D152" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="n">
         <v>10</v>
       </c>
@@ -11935,8 +11977,11 @@
       <c r="C153" s="0" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D153" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="n">
         <v>10</v>
       </c>
@@ -11946,8 +11991,11 @@
       <c r="C154" s="0" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D154" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="n">
         <v>10</v>
       </c>
@@ -11957,8 +12005,11 @@
       <c r="C155" s="0" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D155" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="n">
         <v>10</v>
       </c>
@@ -11968,8 +12019,11 @@
       <c r="C156" s="0" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D156" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="n">
         <v>10</v>
       </c>
@@ -11979,8 +12033,11 @@
       <c r="C157" s="0" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D157" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="n">
         <v>10</v>
       </c>
@@ -11990,8 +12047,11 @@
       <c r="C158" s="0" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D158" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
         <v>10</v>
       </c>
@@ -12001,8 +12061,11 @@
       <c r="C159" s="0" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D159" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
         <v>10</v>
       </c>
@@ -12012,8 +12075,11 @@
       <c r="C160" s="0" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D160" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
         <v>10</v>
       </c>
@@ -12023,8 +12089,11 @@
       <c r="C161" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D161" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="n">
         <v>10</v>
       </c>
@@ -12034,8 +12103,11 @@
       <c r="C162" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D162" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="n">
         <v>10</v>
       </c>
@@ -12044,6 +12116,9 @@
       </c>
       <c r="C163" s="1" t="s">
         <v>184</v>
+      </c>
+      <c r="D163" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12057,7 +12132,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="n">
         <v>10</v>
       </c>
@@ -12067,8 +12142,11 @@
       <c r="C165" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D165" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="n">
         <v>10</v>
       </c>
@@ -12078,8 +12156,11 @@
       <c r="C166" s="0" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D166" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="n">
         <v>10</v>
       </c>
@@ -12089,8 +12170,11 @@
       <c r="C167" s="0" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D167" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="n">
         <v>10</v>
       </c>
@@ -12100,8 +12184,11 @@
       <c r="C168" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D168" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="n">
         <v>10</v>
       </c>
@@ -12111,8 +12198,11 @@
       <c r="C169" s="0" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="170" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D169" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
         <v>10</v>
       </c>
@@ -12122,19 +12212,25 @@
       <c r="C170" s="0" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D170" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B171" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="C171" s="0" t="s">
+      <c r="C171" s="4" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D171" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
         <v>9</v>
       </c>
@@ -12143,6 +12239,9 @@
       </c>
       <c r="C172" s="1" t="s">
         <v>198</v>
+      </c>
+      <c r="D172" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12156,7 +12255,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="n">
         <v>9</v>
       </c>
@@ -12166,8 +12265,11 @@
       <c r="C174" s="0" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D174" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="n">
         <v>9</v>
       </c>
@@ -12177,8 +12279,11 @@
       <c r="C175" s="0" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="176" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D175" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="n">
         <v>9</v>
       </c>
@@ -12188,8 +12293,11 @@
       <c r="C176" s="0" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="177" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D176" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="n">
         <v>9</v>
       </c>
@@ -12199,8 +12307,11 @@
       <c r="C177" s="0" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D177" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="n">
         <v>9</v>
       </c>
@@ -12209,6 +12320,9 @@
       </c>
       <c r="C178" s="0" t="s">
         <v>205</v>
+      </c>
+      <c r="D178" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12222,7 +12336,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="n">
         <v>9</v>
       </c>
@@ -12232,8 +12346,11 @@
       <c r="C180" s="0" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D180" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="n">
         <v>9</v>
       </c>
@@ -12243,8 +12360,11 @@
       <c r="C181" s="0" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D181" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="n">
         <v>9</v>
       </c>
@@ -12254,8 +12374,11 @@
       <c r="C182" s="0" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D182" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="n">
         <v>9</v>
       </c>
@@ -12265,8 +12388,11 @@
       <c r="C183" s="0" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D183" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="n">
         <v>9</v>
       </c>
@@ -12276,8 +12402,11 @@
       <c r="C184" s="0" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D184" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="n">
         <v>9</v>
       </c>
@@ -12287,8 +12416,11 @@
       <c r="C185" s="0" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D185" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="n">
         <v>9</v>
       </c>
@@ -12298,8 +12430,11 @@
       <c r="C186" s="0" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D186" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="n">
         <v>9</v>
       </c>
@@ -12309,8 +12444,11 @@
       <c r="C187" s="0" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="188" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D187" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="n">
         <v>9</v>
       </c>
@@ -12320,8 +12458,11 @@
       <c r="C188" s="0" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D188" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="n">
         <v>9</v>
       </c>
@@ -12331,8 +12472,11 @@
       <c r="C189" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="190" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D189" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="n">
         <v>9</v>
       </c>
@@ -12342,8 +12486,11 @@
       <c r="C190" s="0" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D190" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="n">
         <v>9</v>
       </c>
@@ -12352,6 +12499,9 @@
       </c>
       <c r="C191" s="1" t="s">
         <v>220</v>
+      </c>
+      <c r="D191" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12365,7 +12515,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="n">
         <v>9</v>
       </c>
@@ -12375,8 +12525,11 @@
       <c r="C193" s="0" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="194" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D193" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="n">
         <v>9</v>
       </c>
@@ -12386,8 +12539,11 @@
       <c r="C194" s="0" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="195" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D194" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="n">
         <v>9</v>
       </c>
@@ -12397,8 +12553,11 @@
       <c r="C195" s="0" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="196" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D195" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="n">
         <v>9</v>
       </c>
@@ -12408,8 +12567,11 @@
       <c r="C196" s="0" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="197" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D196" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="n">
         <v>8</v>
       </c>
@@ -12419,8 +12581,11 @@
       <c r="C197" s="0" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="198" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D197" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="n">
         <v>8</v>
       </c>
@@ -12430,8 +12595,11 @@
       <c r="C198" s="0" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="199" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D198" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="n">
         <v>8</v>
       </c>
@@ -12441,8 +12609,11 @@
       <c r="C199" s="0" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="200" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D199" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="n">
         <v>8</v>
       </c>
@@ -12452,8 +12623,11 @@
       <c r="C200" s="0" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="201" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D200" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="n">
         <v>8</v>
       </c>
@@ -12463,8 +12637,11 @@
       <c r="C201" s="0" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="202" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D201" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="n">
         <v>8</v>
       </c>
@@ -12474,8 +12651,11 @@
       <c r="C202" s="0" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D202" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="n">
         <v>8</v>
       </c>
@@ -12485,8 +12665,11 @@
       <c r="C203" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D203" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="n">
         <v>8</v>
       </c>
@@ -12496,8 +12679,11 @@
       <c r="C204" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="205" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D204" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="n">
         <v>8</v>
       </c>
@@ -12507,8 +12693,11 @@
       <c r="C205" s="0" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="206" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D205" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="n">
         <v>8</v>
       </c>
@@ -12518,8 +12707,11 @@
       <c r="C206" s="0" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D206" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="n">
         <v>8</v>
       </c>
@@ -12529,8 +12721,11 @@
       <c r="C207" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D207" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="n">
         <v>8</v>
       </c>
@@ -12540,8 +12735,11 @@
       <c r="C208" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="209" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D208" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="n">
         <v>8</v>
       </c>
@@ -12551,8 +12749,11 @@
       <c r="C209" s="0" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="210" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D209" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="n">
         <v>8</v>
       </c>
@@ -12562,8 +12763,11 @@
       <c r="C210" s="0" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="211" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D210" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="n">
         <v>8</v>
       </c>
@@ -12573,8 +12777,11 @@
       <c r="C211" s="0" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="212" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D211" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="n">
         <v>8</v>
       </c>
@@ -12584,8 +12791,11 @@
       <c r="C212" s="0" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D212" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="n">
         <v>8</v>
       </c>
@@ -12595,8 +12805,11 @@
       <c r="C213" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D213" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="n">
         <v>8</v>
       </c>
@@ -12606,8 +12819,11 @@
       <c r="C214" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D214" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="n">
         <v>8</v>
       </c>
@@ -12617,8 +12833,11 @@
       <c r="C215" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="216" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D215" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="n">
         <v>8</v>
       </c>
@@ -12628,8 +12847,11 @@
       <c r="C216" s="0" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="217" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D216" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="n">
         <v>8</v>
       </c>
@@ -12639,8 +12861,11 @@
       <c r="C217" s="0" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="218" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D217" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="n">
         <v>8</v>
       </c>
@@ -12650,8 +12875,11 @@
       <c r="C218" s="0" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D218" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="n">
         <v>8</v>
       </c>
@@ -12661,8 +12889,11 @@
       <c r="C219" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="220" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D219" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="n">
         <v>8</v>
       </c>
@@ -12672,8 +12903,11 @@
       <c r="C220" s="0" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="221" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D220" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="n">
         <v>8</v>
       </c>
@@ -12683,8 +12917,11 @@
       <c r="C221" s="0" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="222" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D221" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="n">
         <v>8</v>
       </c>
@@ -12694,8 +12931,11 @@
       <c r="C222" s="0" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D222" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="n">
         <v>7</v>
       </c>
@@ -12705,8 +12945,11 @@
       <c r="C223" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="224" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D223" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="n">
         <v>7</v>
       </c>
@@ -12716,8 +12959,11 @@
       <c r="C224" s="0" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="225" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D224" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="n">
         <v>7</v>
       </c>
@@ -12727,8 +12973,11 @@
       <c r="C225" s="0" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="226" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D225" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="n">
         <v>7</v>
       </c>
@@ -12738,8 +12987,11 @@
       <c r="C226" s="0" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="227" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D226" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="n">
         <v>7</v>
       </c>
@@ -12749,8 +13001,11 @@
       <c r="C227" s="0" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="228" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D227" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="n">
         <v>7</v>
       </c>
@@ -12759,6 +13014,9 @@
       </c>
       <c r="C228" s="0" t="s">
         <v>267</v>
+      </c>
+      <c r="D228" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15521,7 +15779,7 @@
       <c r="C479" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="D479" s="4"/>
+      <c r="D479" s="5"/>
     </row>
     <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="0" t="n">
@@ -23285,7 +23543,7 @@
       <c r="B1185" s="0" t="s">
         <v>1471</v>
       </c>
-      <c r="C1185" s="5" t="s">
+      <c r="C1185" s="6" t="s">
         <v>1471</v>
       </c>
     </row>
@@ -23560,7 +23818,7 @@
       <c r="B1210" s="0" t="s">
         <v>1514</v>
       </c>
-      <c r="C1210" s="6" t="s">
+      <c r="C1210" s="7" t="s">
         <v>1514</v>
       </c>
     </row>
@@ -24121,7 +24379,7 @@
       <c r="B1261" s="0" t="s">
         <v>1599</v>
       </c>
-      <c r="C1261" s="7" t="s">
+      <c r="C1261" s="8" t="s">
         <v>1600</v>
       </c>
     </row>

</xml_diff>